<commit_message>
load improved microcode into pc simulation.
the same fibonacci program ran ~12% faster.
</commit_message>
<xml_diff>
--- a/instruction set map.xlsx
+++ b/instruction set map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreas/IdeaProjects/8bit_computer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{721453C8-AD5F-6C4E-9CA4-FE4E3ADCEA01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28172112-D1D2-E34E-99EB-FDD53E67BD56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{835D528E-2EC5-4544-9F35-080965F302CB}"/>
+    <workbookView xWindow="2380" yWindow="6420" windowWidth="35840" windowHeight="21900" xr2:uid="{835D528E-2EC5-4544-9F35-080965F302CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -163,9 +163,6 @@
     <t>BCS i16</t>
   </si>
   <si>
-    <t>BZ i16</t>
-  </si>
-  <si>
     <t>BNZ i16</t>
   </si>
   <si>
@@ -493,10 +490,13 @@
     <t>MOV (SP + i8) CD</t>
   </si>
   <si>
-    <t>RLN</t>
-  </si>
-  <si>
-    <t>RRN</t>
+    <t>RLD</t>
+  </si>
+  <si>
+    <t>RRD</t>
+  </si>
+  <si>
+    <t>BEZ i16</t>
   </si>
 </sst>
 </file>
@@ -911,7 +911,7 @@
   <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="210" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -989,7 +989,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>
@@ -998,23 +998,23 @@
         <v>16</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2" t="s">
         <v>20</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2" t="s">
@@ -1030,7 +1030,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>7</v>
@@ -1039,23 +1039,23 @@
         <v>17</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2" t="s">
         <v>21</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L3" s="2"/>
       <c r="M3" s="2" t="s">
@@ -1071,7 +1071,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>8</v>
@@ -1080,7 +1080,7 @@
         <v>18</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>19</v>
@@ -1090,17 +1090,17 @@
         <v>22</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L4" s="2"/>
       <c r="M4" s="2" t="s">
-        <v>42</v>
+        <v>153</v>
       </c>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
@@ -1112,7 +1112,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>38</v>
@@ -1121,27 +1121,27 @@
         <v>37</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2" t="s">
         <v>23</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L5" s="2"/>
       <c r="M5" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
@@ -1153,36 +1153,36 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>110</v>
-      </c>
       <c r="E6" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2" t="s">
         <v>24</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L6" s="2"/>
       <c r="M6" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
@@ -1194,16 +1194,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -1211,17 +1211,17 @@
         <v>25</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="L7" s="2"/>
       <c r="M7" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
@@ -1233,16 +1233,16 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -1250,17 +1250,17 @@
         <v>26</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="L8" s="2"/>
       <c r="M8" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
@@ -1275,7 +1275,7 @@
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -1283,17 +1283,17 @@
         <v>27</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="L9" s="2"/>
       <c r="M9" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
@@ -1305,36 +1305,36 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2" t="s">
         <v>28</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L10" s="2"/>
       <c r="M10" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
@@ -1346,32 +1346,32 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2" t="s">
         <v>29</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
@@ -1385,36 +1385,36 @@
         <v>0</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2" t="s">
         <v>30</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L12" s="2"/>
       <c r="M12" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
@@ -1426,36 +1426,36 @@
         <v>1</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>39</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2" t="s">
         <v>31</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L13" s="2"/>
       <c r="M13" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
@@ -1467,32 +1467,32 @@
         <v>2</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>114</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2" t="s">
         <v>32</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
@@ -1500,7 +1500,7 @@
       <c r="O14" s="2"/>
       <c r="P14" s="2"/>
       <c r="Q14" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
@@ -1508,32 +1508,32 @@
         <v>3</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2" t="s">
         <v>33</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
@@ -1541,7 +1541,7 @@
       <c r="O15" s="2"/>
       <c r="P15" s="2"/>
       <c r="Q15" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
@@ -1549,13 +1549,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>99</v>
-      </c>
       <c r="D16" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>14</v>
@@ -1566,13 +1566,13 @@
         <v>34</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
@@ -1599,13 +1599,13 @@
         <v>35</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
@@ -1613,7 +1613,7 @@
       <c r="O17" s="2"/>
       <c r="P17" s="2"/>
       <c r="Q17" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
start concept on interrupts
</commit_message>
<xml_diff>
--- a/instruction set map.xlsx
+++ b/instruction set map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreas/IdeaProjects/8bit_computer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28172112-D1D2-E34E-99EB-FDD53E67BD56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3DAA771-6E87-C241-9792-4C32D6F10B5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2380" yWindow="6420" windowWidth="35840" windowHeight="21900" xr2:uid="{835D528E-2EC5-4544-9F35-080965F302CB}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{835D528E-2EC5-4544-9F35-080965F302CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="158">
   <si>
     <t>a</t>
   </si>
@@ -497,6 +497,18 @@
   </si>
   <si>
     <t>BEZ i16</t>
+  </si>
+  <si>
+    <t>INTRPT</t>
+  </si>
+  <si>
+    <t>RETINT</t>
+  </si>
+  <si>
+    <t>NOINT</t>
+  </si>
+  <si>
+    <t>ENINT</t>
   </si>
 </sst>
 </file>
@@ -911,7 +923,7 @@
   <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="210" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1495,7 +1507,9 @@
         <v>147</v>
       </c>
       <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
+      <c r="M14" s="2" t="s">
+        <v>154</v>
+      </c>
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
       <c r="P14" s="2"/>
@@ -1536,7 +1550,9 @@
         <v>148</v>
       </c>
       <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
+      <c r="M15" s="2" t="s">
+        <v>155</v>
+      </c>
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
       <c r="P15" s="2"/>
@@ -1575,7 +1591,9 @@
         <v>149</v>
       </c>
       <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
+      <c r="M16" s="2" t="s">
+        <v>156</v>
+      </c>
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
       <c r="P16" s="2"/>
@@ -1608,7 +1626,9 @@
         <v>150</v>
       </c>
       <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
+      <c r="M17" s="2" t="s">
+        <v>157</v>
+      </c>
       <c r="N17" s="2"/>
       <c r="O17" s="2"/>
       <c r="P17" s="2"/>

</xml_diff>

<commit_message>
simulation and documentation update for interrupts
</commit_message>
<xml_diff>
--- a/instruction set map.xlsx
+++ b/instruction set map.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreas/IdeaProjects/8bit_computer/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\GitHub\8bit_computer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3DAA771-6E87-C241-9792-4C32D6F10B5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B19F2BB9-85E0-467B-9F65-9626839D25E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{835D528E-2EC5-4544-9F35-080965F302CB}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{835D528E-2EC5-4544-9F35-080965F302CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="159">
   <si>
     <t>a</t>
   </si>
@@ -499,16 +499,19 @@
     <t>BEZ i16</t>
   </si>
   <si>
-    <t>INTRPT</t>
-  </si>
-  <si>
-    <t>RETINT</t>
-  </si>
-  <si>
     <t>NOINT</t>
   </si>
   <si>
     <t>ENINT</t>
+  </si>
+  <si>
+    <t>EXINT</t>
+  </si>
+  <si>
+    <t>SIV</t>
+  </si>
+  <si>
+    <t>*INTERRUPT</t>
   </si>
 </sst>
 </file>
@@ -923,30 +926,30 @@
   <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="210" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="15.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="14.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="2.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="2.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="2" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="2.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="2.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="2" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="15.5" style="1"/>
+    <col min="17" max="17" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="15.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B1" s="1">
         <v>0</v>
       </c>
@@ -996,7 +999,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1035,9 +1038,11 @@
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
+      <c r="Q2" s="2" t="s">
+        <v>158</v>
+      </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1076,9 +1081,11 @@
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
+      <c r="Q3" s="2" t="s">
+        <v>156</v>
+      </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1117,9 +1124,11 @@
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
+      <c r="Q4" s="2" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1158,9 +1167,11 @@
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
+      <c r="Q5" s="2" t="s">
+        <v>155</v>
+      </c>
     </row>
-    <row r="6" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1199,9 +1210,11 @@
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
+      <c r="Q6" s="2" t="s">
+        <v>157</v>
+      </c>
     </row>
-    <row r="7" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1240,7 +1253,7 @@
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1279,7 +1292,7 @@
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1312,7 +1325,7 @@
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1353,7 +1366,7 @@
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1392,7 +1405,7 @@
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
@@ -1433,7 +1446,7 @@
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>1</v>
       </c>
@@ -1474,7 +1487,7 @@
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>2</v>
       </c>
@@ -1507,9 +1520,7 @@
         <v>147</v>
       </c>
       <c r="L14" s="2"/>
-      <c r="M14" s="2" t="s">
-        <v>154</v>
-      </c>
+      <c r="M14" s="2"/>
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
       <c r="P14" s="2"/>
@@ -1517,7 +1528,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>3</v>
       </c>
@@ -1550,9 +1561,7 @@
         <v>148</v>
       </c>
       <c r="L15" s="2"/>
-      <c r="M15" s="2" t="s">
-        <v>155</v>
-      </c>
+      <c r="M15" s="2"/>
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
       <c r="P15" s="2"/>
@@ -1560,7 +1569,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>4</v>
       </c>
@@ -1591,9 +1600,7 @@
         <v>149</v>
       </c>
       <c r="L16" s="2"/>
-      <c r="M16" s="2" t="s">
-        <v>156</v>
-      </c>
+      <c r="M16" s="2"/>
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
       <c r="P16" s="2"/>
@@ -1601,7 +1608,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>5</v>
       </c>
@@ -1626,9 +1633,7 @@
         <v>150</v>
       </c>
       <c r="L17" s="2"/>
-      <c r="M17" s="2" t="s">
-        <v>157</v>
-      </c>
+      <c r="M17" s="2"/>
       <c r="N17" s="2"/>
       <c r="O17" s="2"/>
       <c r="P17" s="2"/>

</xml_diff>